<commit_message>
Monitor story is finish
</commit_message>
<xml_diff>
--- a/src/test/java/Resources/mMarktTestCases.xlsx
+++ b/src/test/java/Resources/mMarktTestCases.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="38">
   <si>
     <t>TestID</t>
   </si>
@@ -103,6 +103,42 @@
   <si>
     <t xml:space="preserve">The Samsung page should open
 </t>
+  </si>
+  <si>
+    <t>Then Close cookie window</t>
+  </si>
+  <si>
+    <t>And Click on the Ekranlar from main menu</t>
+  </si>
+  <si>
+    <t>And Click on the Monitör and Monitörleri Keşfedin</t>
+  </si>
+  <si>
+    <t>Then Click on the monitor Ultra Genis</t>
+  </si>
+  <si>
+    <t>And Click on the second monitor</t>
+  </si>
+  <si>
+    <t>3.Close the cookie window when navigate home page</t>
+  </si>
+  <si>
+    <t>4.Click on the Ekranlar from main menu</t>
+  </si>
+  <si>
+    <t>5.Then click on the Monitör and in here select Monitörleri Keşfedin</t>
+  </si>
+  <si>
+    <t>6.After click on the monitor Ultra Genis</t>
+  </si>
+  <si>
+    <t>7.And select the second monitor</t>
+  </si>
+  <si>
+    <t>And Get successfully message</t>
+  </si>
+  <si>
+    <t>8.And get successfully message</t>
   </si>
 </sst>
 </file>
@@ -510,7 +546,7 @@
   <dimension ref="A1:I156"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,33 +636,45 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E4" s="8"/>
+      <c r="E4" s="8" t="s">
+        <v>31</v>
+      </c>
       <c r="F4" s="2"/>
       <c r="G4" s="8"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E5" s="8"/>
+      <c r="E5" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="G5" s="2"/>
       <c r="H5" s="9"/>
     </row>
     <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E6" s="2"/>
+      <c r="E6" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E9" s="2"/>
+      <c r="E9" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
@@ -676,22 +724,34 @@
       </c>
     </row>
     <row r="19" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E19" s="8"/>
+      <c r="E19" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E20" s="2"/>
+      <c r="E20" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E21" s="2"/>
+      <c r="E21" s="2" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E22" s="2"/>
+      <c r="E22" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E23" s="2"/>
+      <c r="E23" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E24" s="2"/>
+      <c r="E24" s="2" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E25" s="2"/>

</xml_diff>